<commit_message>
Use BeanUtils to read model by properties' names getting from excel template
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\POC\ExcelExport\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD9A453-D64E-42FF-BAE6-15BCD6EBCBA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7221767-F8F7-4796-83C4-1942361DF887}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B2A21D7-FC9F-40CA-9902-08B2A6B5950B}"/>
+    <workbookView xWindow="-28920" yWindow="-675" windowWidth="29040" windowHeight="17640" xr2:uid="{9B2A21D7-FC9F-40CA-9902-08B2A6B5950B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Account information</t>
   </si>
@@ -73,13 +73,28 @@
   </si>
   <si>
     <t>Quarter</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>major</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +108,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF9876AA"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -139,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,6 +185,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -508,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925BA35C-F9A7-4E64-B263-11A1FCCEEDF6}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -529,21 +553,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -605,6 +629,23 @@
       <c r="I3" s="1" t="str">
         <f>"Q"&amp;ROUNDUP(MONTH(C3)/3, 0)</f>
         <v>Q4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -613,7 +654,7 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E1:E3 E5:E1048576">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="biology">
       <formula>NOT(ISERROR(SEARCH("biology",E1)))</formula>
     </cfRule>

</xml_diff>